<commit_message>
Update: file xlsx caricati nella repository
</commit_message>
<xml_diff>
--- a/_personale/DB C-Lab (Transfer).xlsx
+++ b/_personale/DB C-Lab (Transfer).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AnagSkill" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Candidati" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AnagSkill" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Candidati" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="AU3" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="AV3" t="n">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="AU4" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="AV4" t="n">

</xml_diff>